<commit_message>
update test case excel (Roby)
</commit_message>
<xml_diff>
--- a/Ujianke6.xlsx
+++ b/Ujianke6.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Java\JUnit\com.juaracoding.courseweek6\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF933BB3-1066-475C-9FFF-F7611852CBC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Executive Summary" sheetId="1" r:id="rId1"/>
@@ -18,17 +19,25 @@
   <externalReferences>
     <externalReference r:id="rId3"/>
   </externalReferences>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="177">
   <si>
     <t>TESTING SUMMARY</t>
   </si>
@@ -388,17 +397,188 @@
   </si>
   <si>
     <t>Jika pass kosong, maka akan tampil notifikasi " Error: Please enter an account password.", sesuai</t>
+  </si>
+  <si>
+    <t>TCC.DC.027</t>
+  </si>
+  <si>
+    <t>TCC.DC.028</t>
+  </si>
+  <si>
+    <t>TCC.DC.029</t>
+  </si>
+  <si>
+    <t>TCC.DC.030</t>
+  </si>
+  <si>
+    <t>TCC.DC.031</t>
+  </si>
+  <si>
+    <t>TCC.DC.032</t>
+  </si>
+  <si>
+    <t>TCC.DC.033</t>
+  </si>
+  <si>
+    <t>TCC.DC.034</t>
+  </si>
+  <si>
+    <t>TCC.DC.035</t>
+  </si>
+  <si>
+    <t>Halaman Search</t>
+  </si>
+  <si>
+    <t>Menampilkan halaman Search</t>
+  </si>
+  <si>
+    <t>Tampail halaman search</t>
+  </si>
+  <si>
+    <t>muncul produk yang di search</t>
+  </si>
+  <si>
+    <t>ROBY</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>tampil halaman product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tampil &amp; sesuai </t>
+  </si>
+  <si>
+    <t>Compare Product</t>
+  </si>
+  <si>
+    <t>memasukkan item produk yang di search</t>
+  </si>
+  <si>
+    <t>Memilih 2 item yang akan di compare</t>
+  </si>
+  <si>
+    <t>tampil &amp; sesuai</t>
+  </si>
+  <si>
+    <t>tampil halaman compare</t>
+  </si>
+  <si>
+    <t>Select option</t>
+  </si>
+  <si>
+    <t>Memilih salah satu produk yang di compare</t>
+  </si>
+  <si>
+    <t>tampil halaman produk yang dipilih</t>
+  </si>
+  <si>
+    <t>Halaman CheckOut</t>
+  </si>
+  <si>
+    <t>Menampilkan halaman Checkout</t>
+  </si>
+  <si>
+    <t>Tampil halaman checkout</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last Name </t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Street Address</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Provincy</t>
+  </si>
+  <si>
+    <t>PostCode</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Terms</t>
+  </si>
+  <si>
+    <t>Place Order</t>
+  </si>
+  <si>
+    <t>TCC.DC.036</t>
+  </si>
+  <si>
+    <t>TCC.DC.037</t>
+  </si>
+  <si>
+    <t>TCC.DC.038</t>
+  </si>
+  <si>
+    <t>TCC.DC.039</t>
+  </si>
+  <si>
+    <t>TCC.DC.040</t>
+  </si>
+  <si>
+    <t>TCC.DC.041</t>
+  </si>
+  <si>
+    <t>TCC.DC.042</t>
+  </si>
+  <si>
+    <t>Mengisi first name</t>
+  </si>
+  <si>
+    <t>Mengisi last name</t>
+  </si>
+  <si>
+    <t>Mengisi country</t>
+  </si>
+  <si>
+    <t>Mengisi City</t>
+  </si>
+  <si>
+    <t>mengisi Provincy</t>
+  </si>
+  <si>
+    <t>Mengisi PostCode</t>
+  </si>
+  <si>
+    <t>Mengisi Phone</t>
+  </si>
+  <si>
+    <t>klik terms</t>
+  </si>
+  <si>
+    <t>klik place order</t>
+  </si>
+  <si>
+    <t>Mengisi secara otomatis</t>
+  </si>
+  <si>
+    <t>centang secara otomatis</t>
+  </si>
+  <si>
+    <t>tampil halaman checkout</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -478,8 +658,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -528,8 +715,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -631,77 +824,14 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -732,22 +862,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -761,9 +876,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -775,12 +887,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -816,37 +922,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -880,6 +956,24 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -889,49 +983,85 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1414,7 +1544,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:N15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1438,127 +1568,127 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="I3" s="3" t="s">
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="I3" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="4">
+      <c r="J3" s="52"/>
+      <c r="K3" s="53">
         <f ca="1">TODAY()</f>
-        <v>44653</v>
-      </c>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
+        <v>44654</v>
+      </c>
+      <c r="L3" s="53"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="53"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="I4" s="3" t="s">
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="I4" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="5">
+      <c r="J4" s="52"/>
+      <c r="K4" s="54">
         <f ca="1">NOW()</f>
-        <v>44653.997854861111</v>
-      </c>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="6"/>
+        <v>44654.459689236108</v>
+      </c>
+      <c r="L4" s="54"/>
+      <c r="M4" s="54"/>
+      <c r="N4" s="2"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="G5" s="7"/>
-      <c r="K5" s="8"/>
+      <c r="G5" s="3"/>
+      <c r="K5" s="4"/>
     </row>
     <row r="6" spans="2:14" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="11"/>
+      <c r="K6" s="7"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B7" s="12">
+      <c r="B7" s="8">
         <v>1</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="9">
         <f>'[1]USER DESKCOLL'!C428</f>
         <v>422</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="9">
         <f>'[1]USER DESKCOLL'!C429</f>
         <v>422</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="9">
         <f>'[1]USER DESKCOLL'!C430</f>
         <v>0</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="10">
         <f>E7/D7*100</f>
         <v>100</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="G8" s="16"/>
+      <c r="G8" s="12"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="13">
         <f>SUM(D7:D7)</f>
         <v>422</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="13">
         <f>SUM(E7:E7)</f>
         <v>422</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="13">
         <f>SUM(F7:F7)</f>
         <v>0</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="11">
         <f>E9/D9*100</f>
         <v>100</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="55"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="G15" s="19"/>
+      <c r="G15" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="D11:G11"/>
     <mergeCell ref="D3:G4"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="K3:N3"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="K4:M4"/>
-    <mergeCell ref="D11:G11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1566,850 +1696,1277 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D6" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13:E14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31:H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" style="42" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" style="43" customWidth="1"/>
-    <col min="3" max="3" width="35.28515625" style="43" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="57" style="44" customWidth="1"/>
-    <col min="5" max="5" width="48" style="44" customWidth="1"/>
-    <col min="6" max="6" width="35.85546875" style="45" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" style="46" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" style="46" customWidth="1"/>
-    <col min="9" max="11" width="7.5703125" style="46" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" style="46" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="46"/>
+    <col min="1" max="1" width="5.5703125" style="30" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="31" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57" style="32" customWidth="1"/>
+    <col min="5" max="5" width="86.28515625" style="32" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.85546875" style="33" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" style="34" customWidth="1"/>
+    <col min="9" max="11" width="7.5703125" style="34" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" style="34" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="34"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="67" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="21"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="68"/>
     </row>
     <row r="3" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="23"/>
+      <c r="A3" s="69"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="70"/>
     </row>
     <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="E4" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="27" t="s">
+      <c r="H4" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="46" t="s">
+      <c r="I4" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="J4" s="46" t="s">
+      <c r="J4" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="K4" s="46" t="s">
+      <c r="K4" s="34" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="47" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="28">
+    <row r="5" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="19">
         <v>1</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="71" t="s">
         <v>69</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="32" t="s">
+      <c r="F5" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="33" t="s">
+      <c r="G5" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="34" t="s">
+      <c r="H5" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="I5" s="46">
+      <c r="I5" s="34">
         <f>IF(G5="Pass",1)</f>
         <v>1</v>
       </c>
-      <c r="J5" s="46" t="b">
+      <c r="J5" s="34" t="b">
         <f t="shared" ref="J5:J14" si="0">IF(G5="Fail",1)</f>
         <v>0</v>
       </c>
-      <c r="K5" s="46" t="b">
+      <c r="K5" s="34" t="b">
         <f t="shared" ref="K5:K14" si="1">IF(G5="(blank)",1)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="45" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="28">
+    <row r="6" spans="1:11" s="33" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A6" s="19">
         <v>2</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="49" t="s">
+      <c r="C6" s="72"/>
+      <c r="D6" s="74"/>
+      <c r="E6" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="F6" s="37" t="s">
+      <c r="F6" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="33" t="s">
+      <c r="G6" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="34" t="s">
+      <c r="H6" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="I6" s="46">
+      <c r="I6" s="34">
         <f t="shared" ref="I6:I14" si="2">IF(G6="Pass",1)</f>
         <v>1</v>
       </c>
-      <c r="J6" s="46" t="b">
+      <c r="J6" s="34" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K6" s="46" t="b">
+      <c r="K6" s="34" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="28">
+      <c r="A7" s="19">
         <v>3</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="D7" s="39" t="s">
+      <c r="D7" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="E7" s="37" t="s">
+      <c r="E7" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="F7" s="37" t="s">
+      <c r="F7" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="33" t="s">
+      <c r="G7" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="34" t="s">
+      <c r="H7" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="I7" s="46">
+      <c r="I7" s="34">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="J7" s="46" t="b">
+      <c r="J7" s="34" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K7" s="46" t="b">
+      <c r="K7" s="34" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="28">
+      <c r="A8" s="19">
         <v>4</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="40" t="s">
+      <c r="D8" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="37" t="s">
+      <c r="E8" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="37" t="s">
+      <c r="F8" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="33" t="s">
+      <c r="G8" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="34" t="s">
+      <c r="H8" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="I8" s="46">
+      <c r="I8" s="34">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="J8" s="46" t="b">
+      <c r="J8" s="34" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K8" s="46" t="b">
+      <c r="K8" s="34" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="28">
+      <c r="A9" s="19">
         <v>5</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="51" t="s">
+      <c r="C9" s="75" t="s">
         <v>71</v>
       </c>
-      <c r="D9" s="52" t="s">
+      <c r="D9" s="76" t="s">
         <v>72</v>
       </c>
-      <c r="E9" s="37" t="s">
+      <c r="E9" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="37" t="s">
+      <c r="F9" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="33" t="s">
+      <c r="G9" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="H9" s="34" t="s">
+      <c r="H9" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="I9" s="46">
+      <c r="I9" s="34">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="J9" s="46" t="b">
+      <c r="J9" s="34" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K9" s="46" t="b">
+      <c r="K9" s="34" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="28">
+      <c r="A10" s="19">
         <v>6</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="51"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="37" t="s">
+      <c r="C10" s="75"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="37" t="s">
+      <c r="F10" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="33" t="s">
+      <c r="G10" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="H10" s="34" t="s">
+      <c r="H10" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="I10" s="46">
+      <c r="I10" s="34">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="J10" s="46" t="b">
+      <c r="J10" s="34" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K10" s="46" t="b">
+      <c r="K10" s="34" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="28">
+      <c r="A11" s="19">
         <v>7</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="51"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="37" t="s">
+      <c r="C11" s="75"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="37" t="s">
+      <c r="F11" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="G11" s="33" t="s">
+      <c r="G11" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="34" t="s">
+      <c r="H11" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="I11" s="46">
+      <c r="I11" s="34">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="J11" s="46" t="b">
+      <c r="J11" s="34" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K11" s="46" t="b">
+      <c r="K11" s="34" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="28">
-        <v>12</v>
-      </c>
-      <c r="B12" s="28" t="s">
+      <c r="A12" s="19">
+        <v>8</v>
+      </c>
+      <c r="B12" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="41" t="s">
+      <c r="C12" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="48" t="s">
+      <c r="D12" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="E12" s="31" t="s">
+      <c r="E12" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="37" t="s">
+      <c r="F12" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="33" t="s">
+      <c r="G12" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="H12" s="34" t="s">
+      <c r="H12" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="I12" s="46">
+      <c r="I12" s="34">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="J12" s="46" t="b">
+      <c r="J12" s="34" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K12" s="46" t="b">
+      <c r="K12" s="34" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="28">
-        <v>13</v>
-      </c>
-      <c r="B13" s="28" t="s">
+      <c r="A13" s="19">
+        <v>9</v>
+      </c>
+      <c r="B13" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="53" t="s">
+      <c r="C13" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="54" t="s">
+      <c r="D13" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="54" t="s">
+      <c r="E13" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="F13" s="54" t="s">
+      <c r="F13" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="G13" s="33" t="s">
+      <c r="G13" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="H13" s="34" t="s">
+      <c r="H13" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="I13" s="46">
+      <c r="I13" s="34">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="J13" s="46" t="b">
+      <c r="J13" s="34" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K13" s="46" t="b">
+      <c r="K13" s="34" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="28">
-        <v>14</v>
-      </c>
-      <c r="B14" s="28" t="s">
+      <c r="A14" s="19">
+        <v>10</v>
+      </c>
+      <c r="B14" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="55"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="33" t="s">
+      <c r="C14" s="66"/>
+      <c r="D14" s="60"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="H14" s="34" t="s">
+      <c r="H14" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="I14" s="46">
+      <c r="I14" s="34">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="J14" s="46" t="b">
+      <c r="J14" s="34" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K14" s="46" t="b">
+      <c r="K14" s="34" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="50">
+      <c r="A15" s="19">
+        <v>11</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="75" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="78" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="F15" s="50" t="s">
+        <v>113</v>
+      </c>
+      <c r="G15" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" s="24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="19">
+        <v>12</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="75"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="G16" s="57"/>
+      <c r="H16" s="24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="19">
+        <v>13</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="75"/>
+      <c r="D17" s="78"/>
+      <c r="E17" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="G17" s="58"/>
+      <c r="H17" s="24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="19">
+        <v>14</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="79" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="78" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="F18" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="G18" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H18" s="24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="19">
         <v>15</v>
       </c>
-      <c r="B15" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="81" t="s">
+      <c r="B19" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="79"/>
+      <c r="D19" s="78"/>
+      <c r="E19" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="G19" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H19" s="24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="19">
+        <v>16</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="79"/>
+      <c r="D20" s="78"/>
+      <c r="E20" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="F20" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="G20" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" s="24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="19">
+        <v>17</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="79"/>
+      <c r="D21" s="78"/>
+      <c r="E21" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="F21" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="G21" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H21" s="24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="19">
+        <v>18</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="79"/>
+      <c r="D22" s="78"/>
+      <c r="E22" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="F22" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="G22" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H22" s="24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="19">
+        <v>19</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="48" t="s">
+        <v>83</v>
+      </c>
+      <c r="D23" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="E23" s="40" t="s">
+        <v>85</v>
+      </c>
+      <c r="F23" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="G23" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H23" s="24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="19">
+        <v>20</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="E24" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="F24" s="43" t="s">
+        <v>90</v>
+      </c>
+      <c r="G24" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H24" s="24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="19">
+        <v>21</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="D25" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="E25" s="43" t="s">
+        <v>93</v>
+      </c>
+      <c r="F25" s="43" t="s">
+        <v>94</v>
+      </c>
+      <c r="G25" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H25" s="24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="19">
+        <v>22</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="46" t="s">
+        <v>95</v>
+      </c>
+      <c r="D26" s="43" t="s">
+        <v>96</v>
+      </c>
+      <c r="E26" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="F26" s="43" t="s">
+        <v>98</v>
+      </c>
+      <c r="G26" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H26" s="24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="19">
+        <v>23</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="61" t="s">
+        <v>99</v>
+      </c>
+      <c r="D27" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="E27" s="43" t="s">
+        <v>101</v>
+      </c>
+      <c r="F27" s="43" t="s">
+        <v>102</v>
+      </c>
+      <c r="G27" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H27" s="24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="19">
+        <v>24</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="62"/>
+      <c r="D28" s="64"/>
+      <c r="E28" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="F28" s="43" t="s">
+        <v>104</v>
+      </c>
+      <c r="G28" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H28" s="24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A29" s="19">
+        <v>25</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="D29" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="E29" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="F29" s="43" t="s">
+        <v>108</v>
+      </c>
+      <c r="G29" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H29" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="I29" s="34"/>
+      <c r="J29" s="34"/>
+      <c r="K29" s="34"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="19">
+        <v>26</v>
+      </c>
+      <c r="B30" s="77" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="D30" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="E30" s="43" t="s">
+        <v>111</v>
+      </c>
+      <c r="F30" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="G30" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H30" s="24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="19">
+        <v>27</v>
+      </c>
+      <c r="B31" s="77" t="s">
+        <v>120</v>
+      </c>
+      <c r="C31" s="80" t="s">
+        <v>129</v>
+      </c>
+      <c r="D31" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="E31" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="F31" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="G31" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="H31" s="83" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="19">
+        <v>28</v>
+      </c>
+      <c r="B32" s="77" t="s">
+        <v>121</v>
+      </c>
+      <c r="C32" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="D32" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="E32" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="F32" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="G32" s="82" t="s">
+        <v>134</v>
+      </c>
+      <c r="H32" s="83" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="19">
+        <v>29</v>
+      </c>
+      <c r="B33" s="77" t="s">
+        <v>122</v>
+      </c>
+      <c r="C33" s="80" t="s">
+        <v>137</v>
+      </c>
+      <c r="D33" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="E33" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="F33" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="G33" s="82" t="s">
+        <v>134</v>
+      </c>
+      <c r="H33" s="83" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="19">
+        <v>30</v>
+      </c>
+      <c r="B34" s="77" t="s">
+        <v>123</v>
+      </c>
+      <c r="C34" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="D34" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="E34" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="F34" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="G34" s="82" t="s">
+        <v>134</v>
+      </c>
+      <c r="H34" s="83" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="19">
+        <v>31</v>
+      </c>
+      <c r="B35" s="77" t="s">
+        <v>124</v>
+      </c>
+      <c r="C35" s="80" t="s">
+        <v>145</v>
+      </c>
+      <c r="D35" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="E35" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="F35" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="G35" s="82" t="s">
+        <v>134</v>
+      </c>
+      <c r="H35" s="83" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="19">
+        <v>32</v>
+      </c>
+      <c r="B36" s="77" t="s">
+        <v>125</v>
+      </c>
+      <c r="C36" s="36" t="s">
+        <v>148</v>
+      </c>
+      <c r="D36" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="E36" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="F36" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="G36" s="82" t="s">
+        <v>134</v>
+      </c>
+      <c r="H36" s="83" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="19">
+        <v>33</v>
+      </c>
+      <c r="B37" s="77" t="s">
+        <v>126</v>
+      </c>
+      <c r="C37" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="D37" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="E37" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="F37" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="G37" s="82" t="s">
+        <v>134</v>
+      </c>
+      <c r="H37" s="83" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="19">
+        <v>34</v>
+      </c>
+      <c r="B38" s="77" t="s">
+        <v>127</v>
+      </c>
+      <c r="C38" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="D38" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="E38" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="F38" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="G38" s="82" t="s">
+        <v>134</v>
+      </c>
+      <c r="H38" s="83" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="19">
+        <v>35</v>
+      </c>
+      <c r="B39" s="77" t="s">
+        <v>128</v>
+      </c>
+      <c r="C39" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="D39" s="81" t="s">
+        <v>167</v>
+      </c>
+      <c r="E39" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="F39" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="G39" s="82" t="s">
+        <v>134</v>
+      </c>
+      <c r="H39" s="83" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="19">
+        <v>36</v>
+      </c>
+      <c r="B40" s="77" t="s">
+        <v>158</v>
+      </c>
+      <c r="C40" s="36" t="s">
+        <v>152</v>
+      </c>
+      <c r="D40" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="E40" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="F40" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="G40" s="82" t="s">
+        <v>134</v>
+      </c>
+      <c r="H40" s="83" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="19">
+        <v>37</v>
+      </c>
+      <c r="B41" s="77" t="s">
+        <v>159</v>
+      </c>
+      <c r="C41" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="D41" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E41" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="F41" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="G41" s="82" t="s">
+        <v>134</v>
+      </c>
+      <c r="H41" s="83" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="19">
+        <v>38</v>
+      </c>
+      <c r="B42" s="77" t="s">
+        <v>160</v>
+      </c>
+      <c r="C42" s="36" t="s">
+        <v>154</v>
+      </c>
+      <c r="D42" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="E42" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="F42" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="G42" s="82" t="s">
+        <v>134</v>
+      </c>
+      <c r="H42" s="83" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="19">
+        <v>39</v>
+      </c>
+      <c r="B43" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="C43" s="36" t="s">
+        <v>155</v>
+      </c>
+      <c r="D43" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="E43" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="F43" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="G43" s="82" t="s">
+        <v>134</v>
+      </c>
+      <c r="H43" s="83" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="19">
+        <v>40</v>
+      </c>
+      <c r="B44" s="77" t="s">
+        <v>162</v>
+      </c>
+      <c r="C44" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="75" t="s">
+      <c r="D44" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="E15" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="F15" s="87" t="s">
-        <v>113</v>
-      </c>
-      <c r="G15" s="72" t="s">
-        <v>4</v>
-      </c>
-      <c r="H15" s="34" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="50">
-        <v>16</v>
-      </c>
-      <c r="B16" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="82"/>
-      <c r="D16" s="76"/>
-      <c r="E16" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="F16" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="G16" s="73"/>
-      <c r="H16" s="34" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="50">
-        <v>17</v>
-      </c>
-      <c r="B17" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="83"/>
-      <c r="D17" s="77"/>
-      <c r="E17" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="F17" s="31" t="s">
-        <v>114</v>
-      </c>
-      <c r="G17" s="74"/>
-      <c r="H17" s="34" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="50"/>
-      <c r="B18" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="78" t="s">
-        <v>74</v>
-      </c>
-      <c r="D18" s="84" t="s">
-        <v>75</v>
-      </c>
-      <c r="E18" s="31" t="s">
-        <v>117</v>
-      </c>
-      <c r="F18" s="31" t="s">
-        <v>117</v>
-      </c>
-      <c r="G18" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="H18" s="34" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="50"/>
-      <c r="B19" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" s="79"/>
-      <c r="D19" s="85"/>
-      <c r="E19" s="31" t="s">
-        <v>77</v>
-      </c>
-      <c r="F19" s="31" t="s">
-        <v>116</v>
-      </c>
-      <c r="G19" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="H19" s="34" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="50"/>
-      <c r="B20" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="79"/>
-      <c r="D20" s="85"/>
-      <c r="E20" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="F20" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="G20" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="H20" s="34" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="50"/>
-      <c r="B21" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="C21" s="79"/>
-      <c r="D21" s="85"/>
-      <c r="E21" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="F21" s="31" t="s">
-        <v>114</v>
-      </c>
-      <c r="G21" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="H21" s="34" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="50"/>
-      <c r="B22" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" s="80"/>
-      <c r="D22" s="86"/>
-      <c r="E22" s="31" t="s">
-        <v>118</v>
-      </c>
-      <c r="F22" s="31" t="s">
-        <v>119</v>
-      </c>
-      <c r="G22" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="H22" s="34" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="50">
-        <v>18</v>
-      </c>
-      <c r="B23" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="C23" s="70" t="s">
-        <v>83</v>
-      </c>
-      <c r="D23" s="69" t="s">
-        <v>84</v>
-      </c>
-      <c r="E23" s="62" t="s">
-        <v>85</v>
-      </c>
-      <c r="F23" s="63" t="s">
-        <v>86</v>
-      </c>
-      <c r="G23" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="H23" s="34" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="50">
-        <v>19</v>
-      </c>
-      <c r="B24" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="C24" s="61" t="s">
-        <v>87</v>
-      </c>
-      <c r="D24" s="66" t="s">
-        <v>88</v>
-      </c>
-      <c r="E24" s="65" t="s">
-        <v>89</v>
-      </c>
-      <c r="F24" s="65" t="s">
-        <v>90</v>
-      </c>
-      <c r="G24" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="H24" s="34" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="50">
-        <v>20</v>
-      </c>
-      <c r="B25" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="C25" s="61" t="s">
-        <v>91</v>
-      </c>
-      <c r="D25" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="E25" s="65" t="s">
-        <v>93</v>
-      </c>
-      <c r="F25" s="65" t="s">
-        <v>94</v>
-      </c>
-      <c r="G25" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="H25" s="34" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="50">
-        <v>21</v>
-      </c>
-      <c r="B26" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26" s="68" t="s">
-        <v>95</v>
-      </c>
-      <c r="D26" s="65" t="s">
-        <v>96</v>
-      </c>
-      <c r="E26" s="65" t="s">
-        <v>97</v>
-      </c>
-      <c r="F26" s="65" t="s">
-        <v>98</v>
-      </c>
-      <c r="G26" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="H26" s="34" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="50">
-        <v>22</v>
-      </c>
-      <c r="B27" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="57" t="s">
-        <v>99</v>
-      </c>
-      <c r="D27" s="59" t="s">
-        <v>100</v>
-      </c>
-      <c r="E27" s="65" t="s">
-        <v>101</v>
-      </c>
-      <c r="F27" s="65" t="s">
-        <v>102</v>
-      </c>
-      <c r="G27" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="H27" s="34" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" s="50">
-        <v>23</v>
-      </c>
-      <c r="B28" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="C28" s="58"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="65" t="s">
-        <v>103</v>
-      </c>
-      <c r="F28" s="65" t="s">
-        <v>104</v>
-      </c>
-      <c r="G28" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="H28" s="34" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" s="44" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A29" s="50">
-        <v>24</v>
-      </c>
-      <c r="B29" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" s="71" t="s">
-        <v>105</v>
-      </c>
-      <c r="D29" s="67" t="s">
-        <v>106</v>
-      </c>
-      <c r="E29" s="62" t="s">
-        <v>107</v>
-      </c>
-      <c r="F29" s="65" t="s">
-        <v>108</v>
-      </c>
-      <c r="G29" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="H29" s="34" t="s">
-        <v>115</v>
-      </c>
-      <c r="I29" s="46"/>
-      <c r="J29" s="46"/>
-      <c r="K29" s="46"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" s="50">
-        <v>25</v>
-      </c>
-      <c r="B30" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="C30" s="61" t="s">
-        <v>109</v>
-      </c>
-      <c r="D30" s="64" t="s">
-        <v>110</v>
-      </c>
-      <c r="E30" s="65" t="s">
-        <v>111</v>
-      </c>
-      <c r="F30" s="65" t="s">
+      <c r="E44" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="F44" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="G44" s="82" t="s">
+        <v>134</v>
+      </c>
+      <c r="H44" s="83" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="19">
+        <v>41</v>
+      </c>
+      <c r="B45" s="77" t="s">
+        <v>163</v>
+      </c>
+      <c r="C45" s="36" t="s">
+        <v>156</v>
+      </c>
+      <c r="D45" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="E45" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="F45" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="G45" s="82" t="s">
+        <v>134</v>
+      </c>
+      <c r="H45" s="83" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="19">
         <v>42</v>
       </c>
-      <c r="G30" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="H30" s="34" t="s">
-        <v>115</v>
+      <c r="B46" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="C46" s="36" t="s">
+        <v>157</v>
+      </c>
+      <c r="D46" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="E46" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="F46" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="G46" s="82" t="s">
+        <v>134</v>
+      </c>
+      <c r="H46" s="83" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="D18:D22"/>
-    <mergeCell ref="C18:C22"/>
+    <mergeCell ref="A2:H3"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="D9:D11"/>
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="D27:D28"/>
     <mergeCell ref="E13:E14"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="D13:D14"/>
-    <mergeCell ref="A2:H3"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="D18:D22"/>
+    <mergeCell ref="C18:C22"/>
   </mergeCells>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
-            <xm:f>'[System Integration Testing(SIT) DESKCOLL V.1 NOV - diluar telephony .xlsx]Parameter'!#REF!</xm:f>
+            <xm:f>'C:\Users\Asus\Downloads\[System Integration Testing(SIT) DESKCOLL V.1 NOV - diluar telephony .xlsx]Parameter'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>G5:G15 G18:G30</xm:sqref>
         </x14:dataValidation>

</xml_diff>